<commit_message>
fixe set assembly bug, update guideline
</commit_message>
<xml_diff>
--- a/zepp_test_command_list_tag0.7.xlsx
+++ b/zepp_test_command_list_tag0.7.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="275">
   <si>
     <t>No.</t>
   </si>
@@ -932,12 +932,6 @@
     <t>check_audio_ready.sh</t>
   </si>
   <si>
-    <t>en_ftm.sh</t>
-  </si>
-  <si>
-    <t>dis_ftm.sh</t>
-  </si>
-  <si>
     <t>./mic_record.sh  &lt;record time in seconds&gt;</t>
   </si>
   <si>
@@ -951,24 +945,6 @@
   </si>
   <si>
     <t>check audio serve and exit when it ready.</t>
-  </si>
-  <si>
-    <t>./en_ftm.sh</t>
-  </si>
-  <si>
-    <t>adb shell /etc/factory-test/zepp/en_ftm.sh</t>
-  </si>
-  <si>
-    <t>enable Wifi/BT FTM mode</t>
-  </si>
-  <si>
-    <t>./dis_ftm.sh</t>
-  </si>
-  <si>
-    <t>adb shell /etc/factory-test/zepp/dis_ftm.sh</t>
-  </si>
-  <si>
-    <t>disable Wifi/BT FTM mode</t>
   </si>
 </sst>
 </file>
@@ -1362,10 +1338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+      <selection activeCell="A77" sqref="A77:XFD77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2102,10 +2078,10 @@
         <v>47</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E45" s="11" t="s">
         <v>172</v>
@@ -2629,47 +2605,13 @@
         <v>269</v>
       </c>
       <c r="C76" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="E76" s="11" t="s">
         <v>274</v>
-      </c>
-      <c r="D76" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="E76" s="11" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
-        <v>76</v>
-      </c>
-      <c r="B77" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="C77" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="D77" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="E77" s="11" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>77</v>
-      </c>
-      <c r="B78" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="C78" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="D78" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="E78" s="11" t="s">
-        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>